<commit_message>
Customer, List, Contract Autonum
Customer, List, Contract Autonum
</commit_message>
<xml_diff>
--- a/RallyLists.xlsx
+++ b/RallyLists.xlsx
@@ -2433,7 +2433,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="60">
+  <cellXfs count="59">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
@@ -2564,12 +2564,6 @@
     <xf numFmtId="0" fontId="6" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="5" borderId="0" xfId="0" quotePrefix="1" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="6" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -2611,6 +2605,9 @@
     </xf>
     <xf numFmtId="0" fontId="13" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="5" borderId="0" xfId="0" quotePrefix="1" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -9461,7 +9458,7 @@
     <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
       <selection activeCell="F1" sqref="F1"/>
-      <selection pane="bottomLeft" activeCell="E16" sqref="E16:E21"/>
+      <selection pane="bottomLeft" activeCell="F8" sqref="F8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -9683,7 +9680,7 @@
       </c>
       <c r="T4" s="36"/>
     </row>
-    <row r="5" spans="1:20" ht="63.75" hidden="1">
+    <row r="5" spans="1:20" ht="63.75">
       <c r="A5" s="36"/>
       <c r="B5" s="36" t="s">
         <v>447</v>
@@ -9730,7 +9727,7 @@
         <v>316</v>
       </c>
     </row>
-    <row r="6" spans="1:20" ht="216.75" hidden="1">
+    <row r="6" spans="1:20" ht="216.75">
       <c r="A6" s="36"/>
       <c r="B6" s="36" t="s">
         <v>447</v>
@@ -9781,7 +9778,7 @@
         <v>316</v>
       </c>
     </row>
-    <row r="7" spans="1:20" ht="25.5" hidden="1">
+    <row r="7" spans="1:20" ht="25.5">
       <c r="A7" s="36"/>
       <c r="B7" s="36" t="s">
         <v>447</v>
@@ -9832,7 +9829,7 @@
         <v>316</v>
       </c>
     </row>
-    <row r="8" spans="1:20" ht="38.25" hidden="1">
+    <row r="8" spans="1:20" ht="38.25">
       <c r="A8" s="36"/>
       <c r="B8" s="36" t="s">
         <v>439</v>
@@ -9884,7 +9881,7 @@
         <v>316</v>
       </c>
     </row>
-    <row r="9" spans="1:20" ht="51" hidden="1">
+    <row r="9" spans="1:20" ht="51">
       <c r="A9" s="36"/>
       <c r="B9" s="36" t="s">
         <v>447</v>
@@ -9934,7 +9931,7 @@
         <v>323</v>
       </c>
     </row>
-    <row r="10" spans="1:20" ht="216.75" hidden="1">
+    <row r="10" spans="1:20">
       <c r="A10" s="36"/>
       <c r="B10" s="36" t="s">
         <v>447</v>
@@ -9945,22 +9942,22 @@
       <c r="D10" s="36" t="s">
         <v>481</v>
       </c>
-      <c r="E10" s="37" t="s">
+      <c r="E10" s="36" t="s">
         <v>212</v>
       </c>
-      <c r="F10" s="37" t="s">
+      <c r="F10" s="36" t="s">
         <v>463</v>
       </c>
-      <c r="G10" s="40" t="s">
+      <c r="G10" s="26" t="s">
         <v>392</v>
       </c>
-      <c r="H10" s="45" t="s">
+      <c r="H10" s="58" t="s">
         <v>485</v>
       </c>
-      <c r="I10" s="42">
+      <c r="I10" s="25">
         <v>1</v>
       </c>
-      <c r="J10" s="42">
+      <c r="J10" s="25">
         <v>1</v>
       </c>
       <c r="K10" s="36" t="s">
@@ -9992,7 +9989,7 @@
         <v>323</v>
       </c>
     </row>
-    <row r="11" spans="1:20" ht="165.75" hidden="1">
+    <row r="11" spans="1:20" ht="165.75">
       <c r="A11" s="36"/>
       <c r="B11" s="36" t="s">
         <v>447</v>
@@ -10050,7 +10047,7 @@
         <v>316</v>
       </c>
     </row>
-    <row r="12" spans="1:20" ht="216.75" hidden="1">
+    <row r="12" spans="1:20" ht="216.75">
       <c r="A12" s="36"/>
       <c r="B12" s="36" t="s">
         <v>447</v>
@@ -10102,7 +10099,7 @@
     </row>
     <row r="13" spans="1:20">
       <c r="A13" s="36"/>
-      <c r="B13" s="56" t="s">
+      <c r="B13" s="54" t="s">
         <v>439</v>
       </c>
       <c r="C13" s="36" t="s">
@@ -10158,7 +10155,7 @@
     </row>
     <row r="14" spans="1:20" ht="38.25">
       <c r="A14" s="36"/>
-      <c r="B14" s="56" t="s">
+      <c r="B14" s="54" t="s">
         <v>447</v>
       </c>
       <c r="C14" s="36" t="s">
@@ -10208,7 +10205,7 @@
     </row>
     <row r="15" spans="1:20" ht="38.25">
       <c r="A15" s="36"/>
-      <c r="B15" s="56" t="s">
+      <c r="B15" s="54" t="s">
         <v>447</v>
       </c>
       <c r="C15" s="36" t="s">
@@ -10252,7 +10249,7 @@
     </row>
     <row r="16" spans="1:20">
       <c r="A16" s="36"/>
-      <c r="B16" s="56" t="s">
+      <c r="B16" s="54" t="s">
         <v>447</v>
       </c>
       <c r="C16" s="36" t="s">
@@ -10304,7 +10301,7 @@
     </row>
     <row r="17" spans="1:20" s="10" customFormat="1" ht="38.25">
       <c r="A17" s="36"/>
-      <c r="B17" s="56" t="s">
+      <c r="B17" s="54" t="s">
         <v>447</v>
       </c>
       <c r="C17" s="36" t="s">
@@ -10354,7 +10351,7 @@
       <c r="A18" s="27">
         <v>7</v>
       </c>
-      <c r="B18" s="57" t="s">
+      <c r="B18" s="55" t="s">
         <v>435</v>
       </c>
       <c r="C18" s="28" t="s">
@@ -10366,11 +10363,11 @@
       <c r="E18" s="29" t="s">
         <v>16</v>
       </c>
-      <c r="F18" s="48" t="s">
+      <c r="F18" s="46" t="s">
         <v>488</v>
       </c>
-      <c r="G18" s="48"/>
-      <c r="H18" s="47" t="s">
+      <c r="G18" s="46"/>
+      <c r="H18" s="45" t="s">
         <v>487</v>
       </c>
       <c r="I18" s="27">
@@ -10402,7 +10399,7 @@
     </row>
     <row r="19" spans="1:20" ht="25.5">
       <c r="A19" s="36"/>
-      <c r="B19" s="56" t="s">
+      <c r="B19" s="54" t="s">
         <v>447</v>
       </c>
       <c r="C19" s="36" t="s">
@@ -10456,7 +10453,7 @@
     </row>
     <row r="20" spans="1:20">
       <c r="A20" s="36"/>
-      <c r="B20" s="56" t="s">
+      <c r="B20" s="54" t="s">
         <v>440</v>
       </c>
       <c r="C20" s="36" t="s">
@@ -10510,7 +10507,7 @@
       <c r="A21" s="27">
         <v>41</v>
       </c>
-      <c r="B21" s="57" t="s">
+      <c r="B21" s="55" t="s">
         <v>439</v>
       </c>
       <c r="C21" s="28" t="s">
@@ -10520,13 +10517,13 @@
       <c r="E21" s="29" t="s">
         <v>86</v>
       </c>
-      <c r="F21" s="50" t="s">
+      <c r="F21" s="48" t="s">
         <v>152</v>
       </c>
-      <c r="G21" s="48" t="s">
+      <c r="G21" s="46" t="s">
         <v>153</v>
       </c>
-      <c r="H21" s="48"/>
+      <c r="H21" s="46"/>
       <c r="I21" s="27">
         <v>3</v>
       </c>
@@ -10558,7 +10555,7 @@
       <c r="A22" s="27">
         <v>12</v>
       </c>
-      <c r="B22" s="58" t="s">
+      <c r="B22" s="56" t="s">
         <v>440</v>
       </c>
       <c r="C22" s="28" t="s">
@@ -10568,11 +10565,11 @@
       <c r="E22" s="29" t="s">
         <v>28</v>
       </c>
-      <c r="F22" s="48" t="s">
+      <c r="F22" s="46" t="s">
         <v>115</v>
       </c>
-      <c r="G22" s="48"/>
-      <c r="H22" s="48" t="s">
+      <c r="G22" s="46"/>
+      <c r="H22" s="46" t="s">
         <v>472</v>
       </c>
       <c r="I22" s="27">
@@ -10606,7 +10603,7 @@
       <c r="A23" s="27">
         <v>13</v>
       </c>
-      <c r="B23" s="58" t="s">
+      <c r="B23" s="56" t="s">
         <v>440</v>
       </c>
       <c r="C23" s="28" t="s">
@@ -10616,11 +10613,11 @@
       <c r="E23" s="29" t="s">
         <v>30</v>
       </c>
-      <c r="F23" s="48" t="s">
+      <c r="F23" s="46" t="s">
         <v>116</v>
       </c>
-      <c r="G23" s="48"/>
-      <c r="H23" s="48"/>
+      <c r="G23" s="46"/>
+      <c r="H23" s="46"/>
       <c r="I23" s="27">
         <v>5</v>
       </c>
@@ -10663,10 +10660,10 @@
       <c r="F24" s="36" t="s">
         <v>290</v>
       </c>
-      <c r="G24" s="49" t="s">
+      <c r="G24" s="47" t="s">
         <v>398</v>
       </c>
-      <c r="H24" s="49"/>
+      <c r="H24" s="47"/>
       <c r="I24" s="38"/>
       <c r="J24" s="38">
         <v>1</v>
@@ -10713,10 +10710,10 @@
       <c r="F25" s="36" t="s">
         <v>289</v>
       </c>
-      <c r="G25" s="49" t="s">
+      <c r="G25" s="47" t="s">
         <v>398</v>
       </c>
-      <c r="H25" s="49"/>
+      <c r="H25" s="47"/>
       <c r="I25" s="38"/>
       <c r="J25" s="38">
         <v>1</v>
@@ -10996,7 +10993,7 @@
         <v>308</v>
       </c>
     </row>
-    <row r="31" spans="1:20" ht="76.5" hidden="1">
+    <row r="31" spans="1:20">
       <c r="A31" s="36"/>
       <c r="B31" s="36" t="s">
         <v>447</v>
@@ -11007,20 +11004,20 @@
       <c r="D31" s="36" t="s">
         <v>482</v>
       </c>
-      <c r="E31" s="37" t="s">
+      <c r="E31" s="36" t="s">
         <v>224</v>
       </c>
-      <c r="F31" s="37" t="s">
+      <c r="F31" s="36" t="s">
         <v>304</v>
       </c>
       <c r="G31" s="26"/>
-      <c r="H31" s="40" t="s">
+      <c r="H31" s="26" t="s">
         <v>486</v>
       </c>
       <c r="I31" s="25">
         <v>1</v>
       </c>
-      <c r="J31" s="46">
+      <c r="J31" s="44">
         <v>1</v>
       </c>
       <c r="K31" s="36" t="s">
@@ -11052,7 +11049,7 @@
         <v>316</v>
       </c>
     </row>
-    <row r="32" spans="1:20" ht="127.5" hidden="1">
+    <row r="32" spans="1:20">
       <c r="A32" s="36"/>
       <c r="B32" s="36" t="s">
         <v>439</v>
@@ -11063,20 +11060,20 @@
       <c r="D32" s="36" t="s">
         <v>482</v>
       </c>
-      <c r="E32" s="37" t="s">
+      <c r="E32" s="36" t="s">
         <v>329</v>
       </c>
-      <c r="F32" s="37" t="s">
+      <c r="F32" s="36" t="s">
         <v>381</v>
       </c>
       <c r="G32" s="26"/>
-      <c r="H32" s="44" t="s">
+      <c r="H32" s="43" t="s">
         <v>483</v>
       </c>
       <c r="I32" s="25">
         <v>1</v>
       </c>
-      <c r="J32" s="46">
+      <c r="J32" s="44">
         <v>1</v>
       </c>
       <c r="K32" s="36" t="s">
@@ -11163,16 +11160,16 @@
         <v>183</v>
       </c>
       <c r="D34" s="36"/>
-      <c r="E34" s="59" t="s">
+      <c r="E34" s="57" t="s">
         <v>184</v>
       </c>
       <c r="F34" s="36" t="s">
         <v>358</v>
       </c>
-      <c r="G34" s="49" t="s">
+      <c r="G34" s="47" t="s">
         <v>398</v>
       </c>
-      <c r="H34" s="49"/>
+      <c r="H34" s="47"/>
       <c r="I34" s="38"/>
       <c r="J34" s="38">
         <v>1</v>
@@ -11221,10 +11218,10 @@
       <c r="F35" s="36" t="s">
         <v>291</v>
       </c>
-      <c r="G35" s="49" t="s">
+      <c r="G35" s="47" t="s">
         <v>378</v>
       </c>
-      <c r="H35" s="49"/>
+      <c r="H35" s="47"/>
       <c r="I35" s="38"/>
       <c r="J35" s="38">
         <v>1</v>
@@ -11256,7 +11253,7 @@
       </c>
       <c r="T35" s="36"/>
     </row>
-    <row r="36" spans="1:20" ht="242.25" hidden="1">
+    <row r="36" spans="1:20">
       <c r="A36" s="36"/>
       <c r="B36" s="36" t="s">
         <v>447</v>
@@ -11267,20 +11264,20 @@
       <c r="D36" s="36" t="s">
         <v>482</v>
       </c>
-      <c r="E36" s="37" t="s">
+      <c r="E36" s="36" t="s">
         <v>176</v>
       </c>
-      <c r="F36" s="37" t="s">
+      <c r="F36" s="36" t="s">
         <v>469</v>
       </c>
       <c r="G36" s="26"/>
-      <c r="H36" s="44" t="s">
+      <c r="H36" s="43" t="s">
         <v>484</v>
       </c>
       <c r="I36" s="25">
         <v>1</v>
       </c>
-      <c r="J36" s="46">
+      <c r="J36" s="44">
         <v>1</v>
       </c>
       <c r="K36" s="36" t="s">
@@ -11312,7 +11309,7 @@
         <v>308</v>
       </c>
     </row>
-    <row r="37" spans="1:20" ht="38.25" hidden="1">
+    <row r="37" spans="1:20" ht="38.25">
       <c r="A37" s="36"/>
       <c r="B37" s="36" t="s">
         <v>447</v>
@@ -11334,7 +11331,7 @@
       <c r="I37" s="25">
         <v>1</v>
       </c>
-      <c r="J37" s="46">
+      <c r="J37" s="44">
         <v>1</v>
       </c>
       <c r="K37" s="36" t="s">
@@ -11964,11 +11961,11 @@
       <c r="E51" s="29" t="s">
         <v>23</v>
       </c>
-      <c r="F51" s="48" t="s">
+      <c r="F51" s="46" t="s">
         <v>112</v>
       </c>
-      <c r="G51" s="51"/>
-      <c r="H51" s="51"/>
+      <c r="G51" s="49"/>
+      <c r="H51" s="49"/>
       <c r="I51" s="27"/>
       <c r="J51" s="27"/>
       <c r="K51" s="27">
@@ -12056,10 +12053,10 @@
       <c r="E53" s="29" t="s">
         <v>60</v>
       </c>
-      <c r="F53" s="48" t="s">
+      <c r="F53" s="46" t="s">
         <v>133</v>
       </c>
-      <c r="G53" s="48"/>
+      <c r="G53" s="46"/>
       <c r="H53" s="26" t="s">
         <v>470</v>
       </c>
@@ -12104,11 +12101,11 @@
       <c r="E54" s="29" t="s">
         <v>58</v>
       </c>
-      <c r="F54" s="48" t="s">
+      <c r="F54" s="46" t="s">
         <v>132</v>
       </c>
-      <c r="G54" s="51"/>
-      <c r="H54" s="51"/>
+      <c r="G54" s="49"/>
+      <c r="H54" s="49"/>
       <c r="I54" s="27"/>
       <c r="J54" s="27"/>
       <c r="K54" s="27">
@@ -12148,11 +12145,11 @@
       <c r="E55" s="29" t="s">
         <v>42</v>
       </c>
-      <c r="F55" s="48" t="s">
+      <c r="F55" s="46" t="s">
         <v>124</v>
       </c>
-      <c r="G55" s="51"/>
-      <c r="H55" s="51"/>
+      <c r="G55" s="49"/>
+      <c r="H55" s="49"/>
       <c r="I55" s="27"/>
       <c r="J55" s="27"/>
       <c r="K55" s="27">
@@ -12242,11 +12239,11 @@
       <c r="E57" s="29" t="s">
         <v>52</v>
       </c>
-      <c r="F57" s="48" t="s">
+      <c r="F57" s="46" t="s">
         <v>129</v>
       </c>
-      <c r="G57" s="48"/>
-      <c r="H57" s="48"/>
+      <c r="G57" s="46"/>
+      <c r="H57" s="46"/>
       <c r="I57" s="27">
         <v>2</v>
       </c>
@@ -12438,7 +12435,7 @@
         <v>432</v>
       </c>
       <c r="G61" s="26"/>
-      <c r="H61" s="48" t="s">
+      <c r="H61" s="46" t="s">
         <v>472</v>
       </c>
       <c r="I61" s="42">
@@ -12488,13 +12485,13 @@
       <c r="E62" s="29" t="s">
         <v>26</v>
       </c>
-      <c r="F62" s="48" t="s">
+      <c r="F62" s="46" t="s">
         <v>113</v>
       </c>
-      <c r="G62" s="51" t="s">
+      <c r="G62" s="49" t="s">
         <v>114</v>
       </c>
-      <c r="H62" s="51"/>
+      <c r="H62" s="49"/>
       <c r="I62" s="27"/>
       <c r="J62" s="27"/>
       <c r="K62" s="27">
@@ -12534,13 +12531,13 @@
       <c r="E63" s="29" t="s">
         <v>66</v>
       </c>
-      <c r="F63" s="48" t="s">
+      <c r="F63" s="46" t="s">
         <v>137</v>
       </c>
-      <c r="G63" s="48" t="s">
+      <c r="G63" s="46" t="s">
         <v>138</v>
       </c>
-      <c r="H63" s="48"/>
+      <c r="H63" s="46"/>
       <c r="I63" s="27">
         <v>3</v>
       </c>
@@ -12630,11 +12627,11 @@
       <c r="E65" s="29" t="s">
         <v>62</v>
       </c>
-      <c r="F65" s="48" t="s">
+      <c r="F65" s="46" t="s">
         <v>134</v>
       </c>
-      <c r="G65" s="51"/>
-      <c r="H65" s="51"/>
+      <c r="G65" s="49"/>
+      <c r="H65" s="49"/>
       <c r="I65" s="27"/>
       <c r="J65" s="27"/>
       <c r="K65" s="27">
@@ -12674,11 +12671,11 @@
       <c r="E66" s="29" t="s">
         <v>74</v>
       </c>
-      <c r="F66" s="48" t="s">
+      <c r="F66" s="46" t="s">
         <v>144</v>
       </c>
-      <c r="G66" s="48"/>
-      <c r="H66" s="48"/>
+      <c r="G66" s="46"/>
+      <c r="H66" s="46"/>
       <c r="I66" s="27">
         <v>3</v>
       </c>
@@ -12768,11 +12765,11 @@
       <c r="E68" s="29" t="s">
         <v>72</v>
       </c>
-      <c r="F68" s="48" t="s">
+      <c r="F68" s="46" t="s">
         <v>143</v>
       </c>
-      <c r="G68" s="48"/>
-      <c r="H68" s="48"/>
+      <c r="G68" s="46"/>
+      <c r="H68" s="46"/>
       <c r="I68" s="27">
         <v>3</v>
       </c>
@@ -12814,11 +12811,11 @@
       <c r="E69" s="29" t="s">
         <v>14</v>
       </c>
-      <c r="F69" s="48" t="s">
+      <c r="F69" s="46" t="s">
         <v>106</v>
       </c>
-      <c r="G69" s="51"/>
-      <c r="H69" s="51"/>
+      <c r="G69" s="49"/>
+      <c r="H69" s="49"/>
       <c r="I69" s="27"/>
       <c r="J69" s="27"/>
       <c r="K69" s="27">
@@ -12858,13 +12855,13 @@
       <c r="E70" s="29" t="s">
         <v>90</v>
       </c>
-      <c r="F70" s="48" t="s">
+      <c r="F70" s="46" t="s">
         <v>156</v>
       </c>
-      <c r="G70" s="48" t="s">
+      <c r="G70" s="46" t="s">
         <v>157</v>
       </c>
-      <c r="H70" s="48"/>
+      <c r="H70" s="46"/>
       <c r="I70" s="27">
         <v>3</v>
       </c>
@@ -12906,11 +12903,11 @@
       <c r="E71" s="34" t="s">
         <v>92</v>
       </c>
-      <c r="F71" s="52" t="s">
+      <c r="F71" s="50" t="s">
         <v>158</v>
       </c>
-      <c r="G71" s="53"/>
-      <c r="H71" s="53"/>
+      <c r="G71" s="51"/>
+      <c r="H71" s="51"/>
       <c r="I71" s="32"/>
       <c r="J71" s="32"/>
       <c r="K71" s="32"/>
@@ -12948,11 +12945,11 @@
       <c r="E72" s="29" t="s">
         <v>46</v>
       </c>
-      <c r="F72" s="48" t="s">
+      <c r="F72" s="46" t="s">
         <v>126</v>
       </c>
-      <c r="G72" s="51"/>
-      <c r="H72" s="51"/>
+      <c r="G72" s="49"/>
+      <c r="H72" s="49"/>
       <c r="I72" s="27"/>
       <c r="J72" s="27"/>
       <c r="K72" s="27"/>
@@ -12990,11 +12987,11 @@
       <c r="E73" s="29" t="s">
         <v>48</v>
       </c>
-      <c r="F73" s="48" t="s">
+      <c r="F73" s="46" t="s">
         <v>127</v>
       </c>
-      <c r="G73" s="51"/>
-      <c r="H73" s="51"/>
+      <c r="G73" s="49"/>
+      <c r="H73" s="49"/>
       <c r="I73" s="27"/>
       <c r="J73" s="27"/>
       <c r="K73" s="27"/>
@@ -13032,11 +13029,11 @@
       <c r="E74" s="29" t="s">
         <v>50</v>
       </c>
-      <c r="F74" s="48" t="s">
+      <c r="F74" s="46" t="s">
         <v>128</v>
       </c>
-      <c r="G74" s="51"/>
-      <c r="H74" s="51"/>
+      <c r="G74" s="49"/>
+      <c r="H74" s="49"/>
       <c r="I74" s="27"/>
       <c r="J74" s="27"/>
       <c r="K74" s="27"/>
@@ -13074,13 +13071,13 @@
       <c r="E75" s="29" t="s">
         <v>84</v>
       </c>
-      <c r="F75" s="48" t="s">
+      <c r="F75" s="46" t="s">
         <v>150</v>
       </c>
-      <c r="G75" s="48" t="s">
+      <c r="G75" s="46" t="s">
         <v>151</v>
       </c>
-      <c r="H75" s="48"/>
+      <c r="H75" s="46"/>
       <c r="I75" s="27">
         <v>3</v>
       </c>
@@ -13122,13 +13119,13 @@
       <c r="E76" s="29" t="s">
         <v>76</v>
       </c>
-      <c r="F76" s="48" t="s">
+      <c r="F76" s="46" t="s">
         <v>145</v>
       </c>
-      <c r="G76" s="48" t="s">
+      <c r="G76" s="46" t="s">
         <v>146</v>
       </c>
-      <c r="H76" s="48"/>
+      <c r="H76" s="46"/>
       <c r="I76" s="27">
         <v>3</v>
       </c>
@@ -13170,13 +13167,13 @@
       <c r="E77" s="29" t="s">
         <v>21</v>
       </c>
-      <c r="F77" s="48" t="s">
+      <c r="F77" s="46" t="s">
         <v>110</v>
       </c>
-      <c r="G77" s="48" t="s">
+      <c r="G77" s="46" t="s">
         <v>111</v>
       </c>
-      <c r="H77" s="48"/>
+      <c r="H77" s="46"/>
       <c r="I77" s="27">
         <v>3</v>
       </c>
@@ -13322,11 +13319,11 @@
       <c r="E80" s="29" t="s">
         <v>1</v>
       </c>
-      <c r="F80" s="48" t="s">
+      <c r="F80" s="46" t="s">
         <v>98</v>
       </c>
-      <c r="G80" s="51"/>
-      <c r="H80" s="51"/>
+      <c r="G80" s="49"/>
+      <c r="H80" s="49"/>
       <c r="I80" s="27"/>
       <c r="J80" s="27"/>
       <c r="K80" s="27">
@@ -13512,13 +13509,13 @@
       <c r="E84" s="29" t="s">
         <v>40</v>
       </c>
-      <c r="F84" s="48" t="s">
+      <c r="F84" s="46" t="s">
         <v>122</v>
       </c>
-      <c r="G84" s="51" t="s">
+      <c r="G84" s="49" t="s">
         <v>123</v>
       </c>
-      <c r="H84" s="51"/>
+      <c r="H84" s="49"/>
       <c r="I84" s="27"/>
       <c r="J84" s="27"/>
       <c r="K84" s="27">
@@ -13854,11 +13851,11 @@
       <c r="E91" s="29" t="s">
         <v>38</v>
       </c>
-      <c r="F91" s="48" t="s">
+      <c r="F91" s="46" t="s">
         <v>121</v>
       </c>
-      <c r="G91" s="51"/>
-      <c r="H91" s="51"/>
+      <c r="G91" s="49"/>
+      <c r="H91" s="49"/>
       <c r="I91" s="27"/>
       <c r="J91" s="27"/>
       <c r="K91" s="27">
@@ -13898,11 +13895,11 @@
       <c r="E92" s="29" t="s">
         <v>78</v>
       </c>
-      <c r="F92" s="48" t="s">
+      <c r="F92" s="46" t="s">
         <v>147</v>
       </c>
-      <c r="G92" s="51"/>
-      <c r="H92" s="51"/>
+      <c r="G92" s="49"/>
+      <c r="H92" s="49"/>
       <c r="I92" s="27"/>
       <c r="J92" s="27"/>
       <c r="K92" s="27">
@@ -13992,11 +13989,11 @@
       <c r="E94" s="29" t="s">
         <v>56</v>
       </c>
-      <c r="F94" s="48" t="s">
+      <c r="F94" s="46" t="s">
         <v>131</v>
       </c>
-      <c r="G94" s="48"/>
-      <c r="H94" s="48"/>
+      <c r="G94" s="46"/>
+      <c r="H94" s="46"/>
       <c r="I94" s="27">
         <v>5</v>
       </c>
@@ -14038,13 +14035,13 @@
       <c r="E95" s="29" t="s">
         <v>64</v>
       </c>
-      <c r="F95" s="48" t="s">
+      <c r="F95" s="46" t="s">
         <v>135</v>
       </c>
-      <c r="G95" s="48" t="s">
+      <c r="G95" s="46" t="s">
         <v>136</v>
       </c>
-      <c r="H95" s="48"/>
+      <c r="H95" s="46"/>
       <c r="I95" s="27">
         <v>5</v>
       </c>
@@ -14134,13 +14131,13 @@
       <c r="E97" s="29" t="s">
         <v>68</v>
       </c>
-      <c r="F97" s="48" t="s">
+      <c r="F97" s="46" t="s">
         <v>139</v>
       </c>
-      <c r="G97" s="51" t="s">
+      <c r="G97" s="49" t="s">
         <v>140</v>
       </c>
-      <c r="H97" s="51"/>
+      <c r="H97" s="49"/>
       <c r="I97" s="27"/>
       <c r="J97" s="27"/>
       <c r="K97" s="27">
@@ -14180,11 +14177,11 @@
       <c r="E98" s="29" t="s">
         <v>54</v>
       </c>
-      <c r="F98" s="48" t="s">
+      <c r="F98" s="46" t="s">
         <v>130</v>
       </c>
-      <c r="G98" s="48"/>
-      <c r="H98" s="48"/>
+      <c r="G98" s="46"/>
+      <c r="H98" s="46"/>
       <c r="I98" s="27">
         <v>5</v>
       </c>
@@ -14226,13 +14223,13 @@
       <c r="E99" s="29" t="s">
         <v>88</v>
       </c>
-      <c r="F99" s="48" t="s">
+      <c r="F99" s="46" t="s">
         <v>154</v>
       </c>
-      <c r="G99" s="51" t="s">
+      <c r="G99" s="49" t="s">
         <v>155</v>
       </c>
-      <c r="H99" s="51"/>
+      <c r="H99" s="49"/>
       <c r="I99" s="27"/>
       <c r="J99" s="27"/>
       <c r="K99" s="27">
@@ -14272,11 +14269,11 @@
       <c r="E100" s="29" t="s">
         <v>5</v>
       </c>
-      <c r="F100" s="48" t="s">
+      <c r="F100" s="46" t="s">
         <v>99</v>
       </c>
-      <c r="G100" s="51"/>
-      <c r="H100" s="51"/>
+      <c r="G100" s="49"/>
+      <c r="H100" s="49"/>
       <c r="I100" s="27"/>
       <c r="J100" s="27"/>
       <c r="K100" s="27">
@@ -14316,11 +14313,11 @@
       <c r="E101" s="29" t="s">
         <v>8</v>
       </c>
-      <c r="F101" s="48" t="s">
+      <c r="F101" s="46" t="s">
         <v>100</v>
       </c>
-      <c r="G101" s="51"/>
-      <c r="H101" s="51"/>
+      <c r="G101" s="49"/>
+      <c r="H101" s="49"/>
       <c r="I101" s="27"/>
       <c r="J101" s="27"/>
       <c r="K101" s="27"/>
@@ -14358,13 +14355,13 @@
       <c r="E102" s="29" t="s">
         <v>10</v>
       </c>
-      <c r="F102" s="48" t="s">
+      <c r="F102" s="46" t="s">
         <v>101</v>
       </c>
-      <c r="G102" s="51" t="s">
+      <c r="G102" s="49" t="s">
         <v>102</v>
       </c>
-      <c r="H102" s="51"/>
+      <c r="H102" s="49"/>
       <c r="I102" s="27"/>
       <c r="J102" s="27"/>
       <c r="K102" s="27"/>
@@ -14404,11 +14401,11 @@
       <c r="E103" s="29" t="s">
         <v>32</v>
       </c>
-      <c r="F103" s="48" t="s">
+      <c r="F103" s="46" t="s">
         <v>117</v>
       </c>
-      <c r="G103" s="51"/>
-      <c r="H103" s="51"/>
+      <c r="G103" s="49"/>
+      <c r="H103" s="49"/>
       <c r="I103" s="27"/>
       <c r="J103" s="27"/>
       <c r="K103" s="27">
@@ -14496,13 +14493,13 @@
       <c r="E105" s="29" t="s">
         <v>12</v>
       </c>
-      <c r="F105" s="48" t="s">
+      <c r="F105" s="46" t="s">
         <v>103</v>
       </c>
-      <c r="G105" s="51" t="s">
+      <c r="G105" s="49" t="s">
         <v>104</v>
       </c>
-      <c r="H105" s="51"/>
+      <c r="H105" s="49"/>
       <c r="I105" s="27"/>
       <c r="J105" s="27"/>
       <c r="K105" s="27">
@@ -14542,13 +14539,13 @@
       <c r="E106" s="29" t="s">
         <v>36</v>
       </c>
-      <c r="F106" s="48" t="s">
+      <c r="F106" s="46" t="s">
         <v>119</v>
       </c>
-      <c r="G106" s="51" t="s">
+      <c r="G106" s="49" t="s">
         <v>120</v>
       </c>
-      <c r="H106" s="51"/>
+      <c r="H106" s="49"/>
       <c r="I106" s="27"/>
       <c r="J106" s="27"/>
       <c r="K106" s="27">
@@ -14636,13 +14633,13 @@
       <c r="E108" s="29" t="s">
         <v>19</v>
       </c>
-      <c r="F108" s="48" t="s">
+      <c r="F108" s="46" t="s">
         <v>108</v>
       </c>
-      <c r="G108" s="51" t="s">
+      <c r="G108" s="49" t="s">
         <v>109</v>
       </c>
-      <c r="H108" s="51"/>
+      <c r="H108" s="49"/>
       <c r="I108" s="27"/>
       <c r="J108" s="27"/>
       <c r="K108" s="27">
@@ -14778,7 +14775,7 @@
       <c r="E111" s="37" t="s">
         <v>310</v>
       </c>
-      <c r="F111" s="49" t="s">
+      <c r="F111" s="47" t="s">
         <v>399</v>
       </c>
       <c r="G111" s="26"/>
@@ -14826,7 +14823,7 @@
       <c r="E112" s="37" t="s">
         <v>312</v>
       </c>
-      <c r="F112" s="49" t="s">
+      <c r="F112" s="47" t="s">
         <v>400</v>
       </c>
       <c r="G112" s="26"/>
@@ -14858,7 +14855,7 @@
         <v>313</v>
       </c>
     </row>
-    <row r="113" spans="1:20" s="4" customFormat="1" ht="25.5" hidden="1">
+    <row r="113" spans="1:20" s="4" customFormat="1" hidden="1">
       <c r="A113" s="27">
         <v>38</v>
       </c>
@@ -14872,11 +14869,11 @@
       <c r="E113" s="29" t="s">
         <v>80</v>
       </c>
-      <c r="F113" s="50" t="s">
+      <c r="F113" s="48" t="s">
         <v>148</v>
       </c>
-      <c r="G113" s="51"/>
-      <c r="H113" s="51"/>
+      <c r="G113" s="49"/>
+      <c r="H113" s="49"/>
       <c r="I113" s="27"/>
       <c r="J113" s="27"/>
       <c r="K113" s="27">
@@ -14916,11 +14913,11 @@
       <c r="E114" s="29" t="s">
         <v>82</v>
       </c>
-      <c r="F114" s="50" t="s">
+      <c r="F114" s="48" t="s">
         <v>149</v>
       </c>
-      <c r="G114" s="51"/>
-      <c r="H114" s="51"/>
+      <c r="G114" s="49"/>
+      <c r="H114" s="49"/>
       <c r="I114" s="27"/>
       <c r="J114" s="27"/>
       <c r="K114" s="27">
@@ -14960,11 +14957,11 @@
       <c r="E115" s="29" t="s">
         <v>44</v>
       </c>
-      <c r="F115" s="48" t="s">
+      <c r="F115" s="46" t="s">
         <v>125</v>
       </c>
-      <c r="G115" s="51"/>
-      <c r="H115" s="51"/>
+      <c r="G115" s="49"/>
+      <c r="H115" s="49"/>
       <c r="I115" s="27"/>
       <c r="J115" s="27"/>
       <c r="K115" s="27">
@@ -15110,11 +15107,11 @@
       <c r="E118" s="29" t="s">
         <v>34</v>
       </c>
-      <c r="F118" s="48" t="s">
+      <c r="F118" s="46" t="s">
         <v>118</v>
       </c>
-      <c r="G118" s="48"/>
-      <c r="H118" s="48" t="s">
+      <c r="G118" s="46"/>
+      <c r="H118" s="46" t="s">
         <v>478</v>
       </c>
       <c r="I118" s="27">
@@ -15157,13 +15154,13 @@
       <c r="E119" s="29" t="s">
         <v>70</v>
       </c>
-      <c r="F119" s="48" t="s">
+      <c r="F119" s="46" t="s">
         <v>141</v>
       </c>
-      <c r="G119" s="51" t="s">
+      <c r="G119" s="49" t="s">
         <v>142</v>
       </c>
-      <c r="H119" s="51"/>
+      <c r="H119" s="49"/>
       <c r="I119" s="27"/>
       <c r="J119" s="27"/>
       <c r="K119" s="27">
@@ -15204,10 +15201,10 @@
       <c r="F120" s="36" t="s">
         <v>298</v>
       </c>
-      <c r="G120" s="54" t="s">
+      <c r="G120" s="52" t="s">
         <v>420</v>
       </c>
-      <c r="H120" s="54"/>
+      <c r="H120" s="52"/>
       <c r="I120" s="41">
         <v>1</v>
       </c>
@@ -15287,7 +15284,7 @@
         <v>308</v>
       </c>
     </row>
-    <row r="122" spans="1:20" ht="25.5">
+    <row r="122" spans="1:20">
       <c r="A122" s="36"/>
       <c r="B122" s="36" t="s">
         <v>450</v>
@@ -15403,9 +15400,9 @@
       <c r="C125" s="17"/>
       <c r="D125" s="17"/>
       <c r="E125" s="1"/>
-      <c r="F125" s="55"/>
-      <c r="G125" s="55"/>
-      <c r="H125" s="55"/>
+      <c r="F125" s="53"/>
+      <c r="G125" s="53"/>
+      <c r="H125" s="53"/>
       <c r="I125" s="17"/>
       <c r="J125" s="17"/>
       <c r="K125" s="17"/>
@@ -15437,9 +15434,9 @@
       <c r="C127" s="17"/>
       <c r="D127" s="17"/>
       <c r="E127" s="1"/>
-      <c r="F127" s="55"/>
-      <c r="G127" s="55"/>
-      <c r="H127" s="55"/>
+      <c r="F127" s="53"/>
+      <c r="G127" s="53"/>
+      <c r="H127" s="53"/>
       <c r="I127" s="17"/>
       <c r="J127" s="17"/>
       <c r="K127" s="17"/>
@@ -15471,9 +15468,9 @@
       <c r="C129" s="17"/>
       <c r="D129" s="17"/>
       <c r="E129" s="1"/>
-      <c r="F129" s="55"/>
-      <c r="G129" s="55"/>
-      <c r="H129" s="55"/>
+      <c r="F129" s="53"/>
+      <c r="G129" s="53"/>
+      <c r="H129" s="53"/>
       <c r="I129" s="17"/>
       <c r="J129" s="17"/>
       <c r="K129" s="17"/>
@@ -15505,9 +15502,9 @@
       <c r="C131" s="17"/>
       <c r="D131" s="17"/>
       <c r="E131" s="1"/>
-      <c r="F131" s="55"/>
-      <c r="G131" s="55"/>
-      <c r="H131" s="55"/>
+      <c r="F131" s="53"/>
+      <c r="G131" s="53"/>
+      <c r="H131" s="53"/>
       <c r="I131" s="17"/>
       <c r="J131" s="17"/>
       <c r="K131" s="17"/>
@@ -15567,11 +15564,6 @@
         <filter val="Order"/>
         <filter val="System"/>
         <filter val="web"/>
-      </filters>
-    </filterColumn>
-    <filterColumn colId="9">
-      <filters blank="1">
-        <filter val="5"/>
       </filters>
     </filterColumn>
   </autoFilter>

</xml_diff>